<commit_message>
Inlude rent index post
</commit_message>
<xml_diff>
--- a/content/post/WhereAreYouFrom/Data/Australia/CensusCountryList_Crosswalk.xlsx
+++ b/content/post/WhereAreYouFrom/Data/Australia/CensusCountryList_Crosswalk.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alastairfraser/Dropbox (Sydney Uni)/Research/Blogs/ImmigrationChanges/Data/Australia/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alastairfraser/Dropbox (Sydney Uni)/Professional/Website/LiveWebsite/Academic_v4/content/post/WhereAreYouFrom/Data/Australia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B8385F-4623-0B4B-96DC-1FE0F2103BE9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA1622C-9BF4-974A-B3A7-7E700167778A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3380" yWindow="4520" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1273" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="708">
   <si>
     <t>CensusCountry</t>
   </si>
@@ -2149,6 +2149,9 @@
   </si>
   <si>
     <t>Syria &amp; Lebanon</t>
+  </si>
+  <si>
+    <t>index</t>
   </si>
 </sst>
 </file>
@@ -2999,9 +3002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D693"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A583" workbookViewId="0">
-      <selection activeCell="B602" sqref="B602"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3009,6 +3010,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>707</v>
+      </c>
       <c r="B1" t="s">
         <v>694</v>
       </c>

</xml_diff>